<commit_message>
Used attribute text; Fixed bug where first flashcard not shown
</commit_message>
<xml_diff>
--- a/Pocket Science/Data Files/Main Data.xlsx
+++ b/Pocket Science/Data Files/Main Data.xlsx
@@ -4697,16 +4697,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4718,7 +4718,7 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4727,7 +4727,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4748,25 +4748,25 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -4991,12 +4991,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -5029,10 +5029,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -5280,12 +5280,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -5600,10 +5600,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>